<commit_message>
Added my name, email, and repo link
</commit_message>
<xml_diff>
--- a/Open Source task.xlsx
+++ b/Open Source task.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\legion\Desktop\open-source\Security-Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mohamed\Security-Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655120EA-671F-4435-B8F2-FC3A0DB523E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{390B0860-0059-4C36-8FC5-6EDC9AC7C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1A782380-5C03-4ABF-949C-B3350E41F3A7}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>Repo Link</t>
   </si>
   <si>
-    <t>https://github.com/0xkillua/Security-Task.git</t>
+    <t>محمد زكي جلال</t>
   </si>
   <si>
-    <t>heikalsayed@gmail.com</t>
+    <t>mohammedzakigalal@gmail.com</t>
   </si>
   <si>
-    <t>السيد اسامه رجب السيد</t>
+    <t>https://github.com/Iammohamedzaki/Security-Task</t>
   </si>
 </sst>
 </file>
@@ -461,7 +461,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -484,13 +484,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>